<commit_message>
site coord QAQC fix and McClung template fix
</commit_message>
<xml_diff>
--- a/ISRaD_Data/McClung_de_Tapia_2005.xlsx
+++ b/ISRaD_Data/McClung_de_Tapia_2005.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="15280" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="15280" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1937" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="1125">
   <si>
     <t>entry_name</t>
   </si>
@@ -3401,6 +3401,9 @@
   </si>
   <si>
     <t>frc_fraction_modern_sd</t>
+  </si>
+  <si>
+    <t>pro_elevation</t>
   </si>
 </sst>
 </file>
@@ -3502,13 +3505,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3520,10 +3535,23 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_layer" xfId="3"/>
   </cellStyles>
@@ -3813,7 +3841,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
@@ -4006,13 +4036,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD21"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -4082,16 +4116,16 @@
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4099,16 +4133,16 @@
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="F5" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4116,16 +4150,16 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="F6" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4133,16 +4167,16 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="F7" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4150,33 +4184,33 @@
         <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" t="s">
-        <v>114</v>
+      <c r="B9" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="F9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4184,13 +4218,13 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="F10" t="s">
         <v>73</v>
@@ -4201,16 +4235,16 @@
         <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -4218,16 +4252,16 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -4235,16 +4269,16 @@
         <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="F13" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4252,16 +4286,16 @@
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4269,16 +4303,16 @@
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="D15" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="F15" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -4286,106 +4320,21 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="C16" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18" t="s">
-        <v>121</v>
-      </c>
-      <c r="F18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" t="s">
-        <v>87</v>
-      </c>
-      <c r="F19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" t="s">
-        <v>127</v>
-      </c>
-      <c r="C21" t="s">
-        <v>128</v>
-      </c>
-      <c r="D21" t="s">
-        <v>129</v>
-      </c>
-      <c r="F21" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A4:G21">
-    <sortCondition ref="C4:C21"/>
+    <sortCondition ref="B4:B21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4399,15 +4348,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ21"/>
+  <dimension ref="A1:AK21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P4" sqref="P4:P21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:37">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4430,94 +4384,97 @@
         <v>135</v>
       </c>
       <c r="H1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="I1" t="s">
         <v>136</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>137</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>138</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>139</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>140</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>141</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>142</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>143</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>144</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>145</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>146</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>147</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>148</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>149</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>150</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>151</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>152</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>153</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>154</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>155</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>156</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>157</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>158</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>159</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>160</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>161</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>162</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>163</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4539,95 +4496,95 @@
       <c r="G2" t="s">
         <v>63</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>168</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>169</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>170</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>171</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>172</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>173</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>174</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>175</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>176</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>177</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>178</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>179</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>180</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>181</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>182</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>183</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>184</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>185</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>186</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>187</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>188</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>189</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>190</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>191</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>192</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>193</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>194</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>195</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4640,44 +4597,41 @@
       <c r="G3" t="s">
         <v>67</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>198</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>199</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>200</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>201</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>36</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>202</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>203</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>204</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>201</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>205</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>206</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>207</v>
-      </c>
-      <c r="V3" t="s">
-        <v>208</v>
       </c>
       <c r="W3" t="s">
         <v>208</v>
@@ -4686,123 +4640,163 @@
         <v>208</v>
       </c>
       <c r="Y3" t="s">
+        <v>208</v>
+      </c>
+      <c r="Z3" t="s">
         <v>209</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>210</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>211</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>212</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>213</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>214</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>205</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>215</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>216</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>217</v>
       </c>
       <c r="AI3" t="s">
         <v>217</v>
       </c>
       <c r="AJ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="AK3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="D4" t="s">
-        <v>218</v>
+        <v>232</v>
+      </c>
+      <c r="F4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" t="s">
+        <v>123</v>
       </c>
       <c r="H4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" t="s">
         <v>219</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>221</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>223</v>
+        <v>237</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" t="s">
+        <v>109</v>
       </c>
       <c r="H5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" t="s">
         <v>219</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>221</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>224</v>
+        <v>231</v>
+      </c>
+      <c r="F6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" t="s">
+        <v>105</v>
       </c>
       <c r="H6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6" t="s">
         <v>219</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>221</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>225</v>
+        <v>224</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" t="s">
+        <v>80</v>
       </c>
       <c r="H7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" t="s">
         <v>219</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>221</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -4812,277 +4806,409 @@
       <c r="D8" t="s">
         <v>226</v>
       </c>
+      <c r="F8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" t="s">
+        <v>112</v>
+      </c>
       <c r="H8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" t="s">
         <v>219</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>221</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>227</v>
+        <v>233</v>
+      </c>
+      <c r="F9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" t="s">
+        <v>87</v>
       </c>
       <c r="H9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I9" t="s">
         <v>219</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>221</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>228</v>
+        <v>236</v>
+      </c>
+      <c r="F10" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" t="s">
+        <v>121</v>
       </c>
       <c r="H10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" t="s">
         <v>219</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>221</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:37">
       <c r="A11" t="s">
         <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="D11" t="s">
-        <v>229</v>
+        <v>239</v>
+      </c>
+      <c r="F11" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" t="s">
+        <v>129</v>
       </c>
       <c r="H11" t="s">
+        <v>130</v>
+      </c>
+      <c r="I11" t="s">
         <v>219</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>221</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:37">
       <c r="A12" t="s">
         <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="D12" t="s">
-        <v>230</v>
+        <v>234</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G12" t="s">
+        <v>116</v>
       </c>
       <c r="H12" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" t="s">
         <v>219</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>221</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:37">
       <c r="A13" t="s">
         <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D13" t="s">
-        <v>231</v>
+        <v>227</v>
+      </c>
+      <c r="F13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" t="s">
+        <v>94</v>
       </c>
       <c r="H13" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" t="s">
         <v>219</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>221</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:37">
       <c r="A14" t="s">
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>232</v>
+        <v>228</v>
+      </c>
+      <c r="F14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" t="s">
+        <v>91</v>
       </c>
       <c r="H14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" t="s">
         <v>219</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>221</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:37">
       <c r="A15" t="s">
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="D15" t="s">
-        <v>233</v>
+        <v>235</v>
+      </c>
+      <c r="F15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" t="s">
+        <v>119</v>
       </c>
       <c r="H15" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" t="s">
         <v>219</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>221</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:37">
       <c r="A16" t="s">
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>234</v>
+        <v>218</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" t="s">
+        <v>72</v>
       </c>
       <c r="H16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" t="s">
         <v>219</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>221</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
         <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>235</v>
+        <v>223</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" t="s">
+        <v>76</v>
       </c>
       <c r="H17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" t="s">
         <v>219</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>221</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>236</v>
+        <v>225</v>
+      </c>
+      <c r="F18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" t="s">
+        <v>84</v>
       </c>
       <c r="H18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" t="s">
         <v>219</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>221</v>
       </c>
-      <c r="U18" t="s">
+      <c r="V18" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:22">
       <c r="A19" t="s">
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D19" t="s">
-        <v>237</v>
+        <v>230</v>
+      </c>
+      <c r="F19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" t="s">
+        <v>101</v>
       </c>
       <c r="H19" t="s">
+        <v>102</v>
+      </c>
+      <c r="I19" t="s">
         <v>219</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
         <v>221</v>
       </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>238</v>
+        <v>229</v>
+      </c>
+      <c r="F20" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" t="s">
+        <v>97</v>
       </c>
       <c r="H20" t="s">
+        <v>98</v>
+      </c>
+      <c r="I20" t="s">
         <v>219</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
         <v>221</v>
       </c>
-      <c r="U20" t="s">
+      <c r="V20" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D21" t="s">
-        <v>239</v>
+        <v>238</v>
+      </c>
+      <c r="F21" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" t="s">
+        <v>126</v>
       </c>
       <c r="H21" t="s">
+        <v>113</v>
+      </c>
+      <c r="I21" t="s">
         <v>219</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>221</v>
       </c>
-      <c r="U21" t="s">
+      <c r="V21" t="s">
         <v>222</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A4:AK21">
+    <sortCondition ref="B4:B21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
@@ -5419,11 +5545,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CT69"/>
   <sheetViews>
-    <sheetView topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="AZ4" sqref="AZ4:BA92"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:98">
       <c r="A1" t="s">
@@ -8618,7 +8748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="AI1" sqref="AI1:AK1"/>
     </sheetView>
   </sheetViews>

</xml_diff>